<commit_message>
Updated sheet with qtbrowser releases
</commit_message>
<xml_diff>
--- a/projects/Commitnumbers.xlsx
+++ b/projects/Commitnumbers.xlsx
@@ -5,17 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="356" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Customer</t>
   </si>
@@ -67,6 +72,33 @@
   <si>
     <t>First qt5.4.1 delivery to Pace as part of the S1b build within the Dawn project
 (http://download.qt.io/official_releases/qt/5.4/5.4.1/submodules/)</t>
+  </si>
+  <si>
+    <t>qtbrowser-2.0.9</t>
+  </si>
+  <si>
+    <t>a3e844872639992072f8f81830f67e8a56a592f0</t>
+  </si>
+  <si>
+    <t>enabled websecurity</t>
+  </si>
+  <si>
+    <t>qtbrowser-2.0.10</t>
+  </si>
+  <si>
+    <t>10c09a0589129af0f9b5963f719ed6fa2790e922</t>
+  </si>
+  <si>
+    <t>Conditionally added syslog functionality</t>
+  </si>
+  <si>
+    <t>qtbrowser-2.0.11</t>
+  </si>
+  <si>
+    <t>7193f983d5a07207a67dd22ec0ef0877b885e4fc</t>
+  </si>
+  <si>
+    <t>Fixed syslog issue</t>
   </si>
 </sst>
 </file>
@@ -184,20 +216,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.662962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.162962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.2"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.2407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="99.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.8333333333333"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -265,7 +296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -282,9 +313,60 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" display="http://download.qt.io/official_releases/qt/5.4/5.4.1/submodules/"/>
+    <hyperlink ref="E6" r:id="rId1" display="First qt5.4.1 delivery to Pace as part of the S1b build within the Dawn project&#10;(http://download.qt.io/official_releases/qt/5.4/5.4.1/submodules/)"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Updated overview with new PACE delivery for Dawn
</commit_message>
<xml_diff>
--- a/projects/Commitnumbers.xlsx
+++ b/projects/Commitnumbers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Customer</t>
   </si>
@@ -99,6 +99,19 @@
   </si>
   <si>
     <t>Fixed syslog issue</t>
+  </si>
+  <si>
+    <t>QtBrowser
+qtbrowser-2.0.11
+qtwebkit-5.4.1</t>
+  </si>
+  <si>
+    <t>
+7193f983d5a07207a67dd22ec0ef0877b885e4fc
+bf14b0e5b3178efe9326df8cb4a3c21214199cd5</t>
+  </si>
+  <si>
+    <t>Extended syslog support by allowing (optional) redirect qtbrowser output to syslog instead of console (define QT_BUILD_WITH_SYSLOG for syslog support)</t>
   </si>
 </sst>
 </file>
@@ -216,19 +229,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.2407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="99.3666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.75555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.4444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="102.388888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.0481481481481"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,6 +376,23 @@
       </c>
       <c r="E9" s="0" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>